<commit_message>
UPD Documentos 20230421 1158
</commit_message>
<xml_diff>
--- a/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Servicios/Citas - Telemarketing/Toyota - CEL - Analisis - Servicio - Citas_CRT - v1_1_1 - Parte de CRT No esta Implementada Formalmente.xlsx
+++ b/TOYOTA-Celaya/Fuentes - Toyota/Distribuidor/Servicios/Citas - Telemarketing/Toyota - CEL - Analisis - Servicio - Citas_CRT - v1_1_1 - Parte de CRT No esta Implementada Formalmente.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KE\JMM\PROCESSES MAPPING\TOYOTA - Celaya\Fuentes - Toyota\Distribuidor\Servicios\Citas - Telemarketing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KE\JMM\PROCESSES MAPPING\toyota_proceso\TOYOTA-Celaya\Fuentes - Toyota\Distribuidor\Servicios\Citas - Telemarketing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE4B9579-8013-46D0-8875-BBE6B3AA05C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2771E08B-5A54-47DF-A34C-67F56B08EAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="465" yWindow="330" windowWidth="19950" windowHeight="10530" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
+    <workbookView xWindow="270" yWindow="75" windowWidth="19950" windowHeight="10800" xr2:uid="{7E74557B-02A4-44EF-8F45-FC026D5565D6}"/>
   </bookViews>
   <sheets>
     <sheet name="FTO Task List" sheetId="4" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="335">
   <si>
     <t>Tipo</t>
   </si>
@@ -686,17 +686,6 @@
     <t>Archivos adjuntos</t>
   </si>
   <si>
-    <t>Campos que no se tienen en Kepler.
-- Domicilio de recolección de Unidad (campos específicos)
-- Contacto para la recolección
-- Horario de recolección
-- Fecha de recolección
-- No se cuenta con información de Acciones de Servicio pendientes (campañas)
-- Campos telefónicos deben ser numéricos y de 10 dígitos.
-- En Historial del cliente no se puede visualizar toda la información de la orden, tenemos que salir y abrir la orden. En el historial deseamos ver los comentarios completos de la orden sin salir de la pantalla.
-- En la asignación del técnico sólo se ve la clave y el nombre no el nivel del técnico (su rol)</t>
-  </si>
-  <si>
     <t>REPORTE DE CITAS  Y NO SHOW .XLSX</t>
   </si>
   <si>
@@ -714,13 +703,6 @@
   <si>
     <t>Que el control no sea manual sino desde el sistema, incluido el 20% de provisionamiento para los Sin Cita, incluyendo el código de colores (especificado en la guía)
 Poder gestionar desde el sistema disponibilidad de los técnicos y/o Asesores de Servicio, esto también debería incluirse para el cálculo del 20% de disponibilidad.</t>
-  </si>
-  <si>
-    <t>Campos que no se tienen en Kepler.
-- Domicilio para servicio móvil (campos específicos)
-- Contacto para la ubicación
-- Horario
-- Gestionar con estatus disponibilidad de los técnicos y/o con agenda</t>
   </si>
   <si>
     <t>Actualmente sólo contamos con 3 perfiles en el sistema, falta el del propietario</t>
@@ -1510,6 +1492,142 @@
     <t>ID Task</t>
   </si>
   <si>
+    <t>V - Ventas
+S - Servicio</t>
+  </si>
+  <si>
+    <t>A - A,B,C
+V - View</t>
+  </si>
+  <si>
+    <t>K - K75
+T - Toyota
+D - DISTR</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Type Aux</t>
+  </si>
+  <si>
+    <t>TBL - Entity</t>
+  </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>K75</t>
+  </si>
+  <si>
+    <t>K75 - Ref</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>APP - Ref</t>
+  </si>
+  <si>
+    <t>TOY</t>
+  </si>
+  <si>
+    <t>TOY Ref</t>
+  </si>
+  <si>
+    <t>DISTR</t>
+  </si>
+  <si>
+    <t>DISTR - Ref</t>
+  </si>
+  <si>
+    <t>DMS</t>
+  </si>
+  <si>
+    <t>Cobertura</t>
+  </si>
+  <si>
+    <t>DMS - Ref</t>
+  </si>
+  <si>
+    <t>CPU's</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crecimiento en CPU's del 8% en comparación con el mismo mes del año anterior. </t>
+  </si>
+  <si>
+    <t>XLS REF : 
+S - C - ID Task</t>
+  </si>
+  <si>
+    <t>S - C - 001</t>
+  </si>
+  <si>
+    <t>Los campos que no llenan: 
+- Código Katashiki
+- Fecha Dofu
+- Garantía Extendida (fecha de vigencia)
+- Seguro Vehicular
+- Transmisión
+La idea es restringir captura de transacciones por falta de estos datos en algunos casos
+- Fecha de entrega de la unidad (para Toyota la fecha DOFU es la que rige la programación de servicio)</t>
+  </si>
+  <si>
+    <t>Disponibilidad de los campos necesarios en el DMS (sistema operativo) para registrar la información del historial de servicio derivada
+de las citas.</t>
+  </si>
+  <si>
+    <t>Domicilio Recoleccion</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>Contacto Recoleccion</t>
+  </si>
+  <si>
+    <t>Separar por campos ( calle, numero ext., numero int. colonia, ciudad, etc. ), modalidad de recoleccion de Auto del Cliente</t>
+  </si>
+  <si>
+    <t>Para modalidad de recoleccion del Auto del Cliente</t>
+  </si>
+  <si>
+    <t>A, V</t>
+  </si>
+  <si>
+    <t>Horario Recoleccion</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>Fecha Recoleccion</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>K-CI-1</t>
+  </si>
+  <si>
+    <t>Informacion de Campañas</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
     <t>T - Texto
 N - Entero
 D - Decimal
@@ -1518,104 +1636,105 @@
 FH - F &amp; H
 S - Flag / ST
 C - Catalogo
-R - Control</t>
-  </si>
-  <si>
-    <t>V - Ventas
-S - Servicio</t>
-  </si>
-  <si>
-    <t>A - A,B,C
-V - View</t>
-  </si>
-  <si>
-    <t>K - K75
-T - Toyota
-D - DISTR</t>
-  </si>
-  <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Type Aux</t>
-  </si>
-  <si>
-    <t>TBL - Entity</t>
-  </si>
-  <si>
-    <t>Module</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Usage</t>
-  </si>
-  <si>
-    <t>Mandatory</t>
-  </si>
-  <si>
-    <t>K75</t>
-  </si>
-  <si>
-    <t>K75 - Ref</t>
-  </si>
-  <si>
-    <t>APP</t>
-  </si>
-  <si>
-    <t>APP - Ref</t>
-  </si>
-  <si>
-    <t>TOY</t>
-  </si>
-  <si>
-    <t>TOY Ref</t>
-  </si>
-  <si>
-    <t>DISTR</t>
-  </si>
-  <si>
-    <t>DISTR - Ref</t>
-  </si>
-  <si>
-    <t>DMS</t>
-  </si>
-  <si>
-    <t>Cobertura</t>
-  </si>
-  <si>
-    <t>DMS - Ref</t>
-  </si>
-  <si>
-    <t>CPU's</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crecimiento en CPU's del 8% en comparación con el mismo mes del año anterior. </t>
-  </si>
-  <si>
-    <t>XLS REF : 
-S - C - ID Task</t>
-  </si>
-  <si>
-    <t>S - C - 001</t>
-  </si>
-  <si>
-    <t>Los campos que no llenan: 
-- Código Katashiki
-- Fecha Dofu
-- Garantía Extendida (fecha de vigencia)
-- Seguro Vehicular
-- Transmisión
-La idea es restringir captura de transacciones por falta de estos datos en algunos casos
-- Fecha de entrega de la unidad (para Toyota la fecha DOFU es la que rige la programación de servicio)</t>
-  </si>
-  <si>
-    <t>Disponibilidad de los campos necesarios en el DMS (sistema operativo) para registrar la información del historial de servicio derivada
-de las citas.</t>
+R - Control (Conjunto de Datos incluidos en un proceso )</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Clientes, Autos, Campañas</t>
+  </si>
+  <si>
+    <t>Una opcion para Visualizar las Campañas Activas de un Modelo asociado a un Cliente, incluida Descripcion.</t>
+  </si>
+  <si>
+    <t>Numeros Telenicos</t>
+  </si>
+  <si>
+    <t>Se solicita que los Numeros Telefonicos sean de 10 Digitos. Analizar Alcance, Toyota si les envia un Reporte donde identica estos datos como Incorrectos.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Campos que no se tienen en Kepler.
+- Domicilio de recolección de Unidad (campos específicos)
+- Contacto para la recolección
+- Horario de recolección
+- Fecha de recolección
+- No se cuenta con información de Acciones de Servicio pendientes (campañas)
+- Campos telefónicos deben ser numéricos y de 10 dígitos.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- En Historial del cliente no se puede visualizar toda la información de la orden, tenemos que salir y abrir la orden. En el historial deseamos ver los comentarios completos de la orden sin salir de la pantalla.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- En la asignación del técnico sólo se ve la clave y el nombre no el nivel del técnico (su rol)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Campos que no se tienen en Kepler.
+- Domicilio para servicio móvil (campos específicos)
+- Contacto para la ubicación
+- Horario
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Gestionar con estatus disponibilidad de los técnicos y/o con agenda ( Que se tengan para asignar solo las Hrs. Habiles de los Tecnicos, gestionando las Hrs. de Vacaciones, Cursos, Comidas, Permisos, como No Disponibles para No Asignarles Trabajos ).</t>
+    </r>
+  </si>
+  <si>
+    <t>S - C - 002</t>
+  </si>
+  <si>
+    <t>Domicilio SERV Movil</t>
+  </si>
+  <si>
+    <t>Contacto SERV Movil</t>
+  </si>
+  <si>
+    <t>Horario SERV Movil</t>
+  </si>
+  <si>
+    <t>Fecha SERV Movil</t>
+  </si>
+  <si>
+    <t>Separar por campos ( calle, numero ext., numero int. colonia, ciudad, etc. ), modalidad de SERV Movil para  Auto del Cliente. Se puede Homologar un Esquema de Datos Alternativos que se usen para SERV Movil y Recoleccion de acuerdo al Tipo de Servicio / Orden.</t>
+  </si>
+  <si>
+    <t>Para modalidad de recoleccion del Auto del Cliente. Se puede Homologar un Esquema de Datos Alternativos que se usen para SERV Movil y Recoleccion de acuerdo al Tipo de Servicio / Orden.</t>
   </si>
 </sst>
 </file>
@@ -2365,10 +2484,10 @@
   <dimension ref="B2:AB46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <pane xSplit="6" ySplit="4" topLeftCell="Y11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="4" topLeftCell="G6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="G1" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Y11" sqref="Y11"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2513,7 @@
     <col min="19" max="19" width="20.7109375" style="2" customWidth="1"/>
     <col min="20" max="20" width="15.85546875" style="2" customWidth="1"/>
     <col min="21" max="21" width="35.5703125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17.5703125" style="2" customWidth="1"/>
     <col min="23" max="23" width="35.42578125" style="2" customWidth="1"/>
     <col min="24" max="24" width="27.140625" style="2" customWidth="1"/>
     <col min="25" max="25" width="24.42578125" style="2" customWidth="1"/>
@@ -2404,7 +2523,7 @@
     <col min="29" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:28" s="1" customFormat="1" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>62</v>
       </c>
@@ -2453,7 +2572,7 @@
         <v>30</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="3" spans="2:28" ht="18.75" x14ac:dyDescent="0.25">
@@ -2575,7 +2694,7 @@
         <v>127</v>
       </c>
       <c r="AB4" s="6" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="5" spans="2:28" ht="263.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -2621,18 +2740,18 @@
         <v>68</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R5" s="24"/>
       <c r="S5" s="34" t="s">
         <v>69</v>
       </c>
       <c r="T5" s="34" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="U5" s="34"/>
       <c r="V5" s="34" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="W5" s="34" t="s">
         <v>70</v>
@@ -2642,13 +2761,13 @@
       </c>
       <c r="Y5" s="34"/>
       <c r="Z5" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="AA5" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="AA5" s="5" t="s">
-        <v>129</v>
-      </c>
       <c r="AB5" s="7" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2694,7 +2813,7 @@
         <v>75</v>
       </c>
       <c r="Q6" s="24" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="R6" s="24"/>
       <c r="S6" s="34" t="s">
@@ -2704,17 +2823,19 @@
       <c r="U6" s="34"/>
       <c r="V6" s="34"/>
       <c r="W6" s="34" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="X6" s="34" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="Y6" s="34"/>
       <c r="Z6" s="5" t="s">
-        <v>134</v>
+        <v>327</v>
       </c>
       <c r="AA6" s="5"/>
-      <c r="AB6" s="7"/>
+      <c r="AB6" s="7" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="7" spans="2:28" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="32" t="s">
@@ -2759,7 +2880,7 @@
         <v>77</v>
       </c>
       <c r="Q7" s="24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="R7" s="24"/>
       <c r="S7" s="34"/>
@@ -2770,7 +2891,7 @@
       <c r="X7" s="34"/>
       <c r="Y7" s="34"/>
       <c r="Z7" s="5" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AA7" s="5"/>
       <c r="AB7" s="7"/>
@@ -2816,7 +2937,7 @@
         <v>80</v>
       </c>
       <c r="Q8" s="24" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R8" s="24"/>
       <c r="S8" s="34" t="s">
@@ -2833,7 +2954,7 @@
       </c>
       <c r="Y8" s="34"/>
       <c r="Z8" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AA8" s="5"/>
       <c r="AB8" s="7"/>
@@ -2892,7 +3013,7 @@
       <c r="X9" s="34"/>
       <c r="Y9" s="34"/>
       <c r="Z9" s="5" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="AA9" s="5"/>
       <c r="AB9" s="7"/>
@@ -3000,10 +3121,10 @@
         <v>72</v>
       </c>
       <c r="P11" s="24" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="Q11" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="R11" s="24"/>
       <c r="S11" s="34"/>
@@ -3014,10 +3135,10 @@
       <c r="X11" s="34"/>
       <c r="Y11" s="34"/>
       <c r="Z11" s="5" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="AA11" s="5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="AB11" s="7"/>
     </row>
@@ -3061,10 +3182,10 @@
         <v>72</v>
       </c>
       <c r="P12" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q12" s="24" t="s">
         <v>142</v>
-      </c>
-      <c r="Q12" s="24" t="s">
-        <v>144</v>
       </c>
       <c r="R12" s="24"/>
       <c r="S12" s="34"/>
@@ -3075,7 +3196,7 @@
       <c r="X12" s="34"/>
       <c r="Y12" s="34"/>
       <c r="Z12" s="5" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="AA12" s="5"/>
       <c r="AB12" s="7"/>
@@ -3120,10 +3241,10 @@
         <v>72</v>
       </c>
       <c r="P13" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="Q13" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="R13" s="24"/>
       <c r="S13" s="34"/>
@@ -3134,7 +3255,7 @@
       <c r="X13" s="34"/>
       <c r="Y13" s="34"/>
       <c r="Z13" s="5" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="AA13" s="5"/>
       <c r="AB13" s="7"/>
@@ -3173,7 +3294,7 @@
       </c>
       <c r="M14" s="24"/>
       <c r="N14" s="24" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="O14" s="24" t="s">
         <v>72</v>
@@ -3193,7 +3314,7 @@
       <c r="X14" s="34"/>
       <c r="Y14" s="34"/>
       <c r="Z14" s="5" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="AA14" s="5"/>
       <c r="AB14" s="7"/>
@@ -3302,23 +3423,23 @@
       </c>
       <c r="R16" s="24"/>
       <c r="S16" s="34" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="T16" s="34"/>
       <c r="U16" s="34"/>
       <c r="V16" s="34"/>
       <c r="W16" s="34" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="X16" s="34" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="Y16" s="34"/>
       <c r="Z16" s="5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AA16" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AB16" s="7"/>
     </row>
@@ -3362,10 +3483,10 @@
         <v>72</v>
       </c>
       <c r="P17" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="Q17" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="R17" s="24"/>
       <c r="S17" s="34"/>
@@ -3373,17 +3494,17 @@
       <c r="U17" s="34"/>
       <c r="V17" s="34"/>
       <c r="W17" s="34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="X17" s="34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Y17" s="34"/>
       <c r="Z17" s="5" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="AA17" s="5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AB17" s="7"/>
     </row>
@@ -3433,7 +3554,7 @@
         <v>105</v>
       </c>
       <c r="R18" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="S18" s="34"/>
       <c r="T18" s="34"/>
@@ -3491,7 +3612,7 @@
         <v>114</v>
       </c>
       <c r="Q19" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="R19" s="24"/>
       <c r="S19" s="34"/>
@@ -3502,10 +3623,10 @@
       <c r="X19" s="34"/>
       <c r="Y19" s="34"/>
       <c r="Z19" s="5" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="AA19" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB19" s="7"/>
     </row>
@@ -3551,7 +3672,7 @@
         <v>67</v>
       </c>
       <c r="P20" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="Q20" s="24" t="s">
         <v>119</v>
@@ -3565,10 +3686,10 @@
       <c r="X20" s="34"/>
       <c r="Y20" s="34"/>
       <c r="Z20" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="AA20" s="5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="AB20" s="7"/>
     </row>
@@ -3613,7 +3734,7 @@
         <v>122</v>
       </c>
       <c r="Q21" s="24" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="R21" s="24"/>
       <c r="S21" s="34"/>
@@ -3626,10 +3747,10 @@
       <c r="X21" s="34"/>
       <c r="Y21" s="34"/>
       <c r="Z21" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="AA21" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AB21" s="7"/>
     </row>
@@ -3663,7 +3784,7 @@
         <v>60</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="M22" s="24" t="s">
         <v>57</v>
@@ -3691,10 +3812,10 @@
       <c r="X22" s="34"/>
       <c r="Y22" s="34"/>
       <c r="Z22" s="5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="AA22" s="5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AB22" s="7"/>
     </row>
@@ -3706,7 +3827,7 @@
         <v>15</v>
       </c>
       <c r="D23" s="32" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E23" s="32"/>
       <c r="F23" s="32" t="s">
@@ -3719,25 +3840,25 @@
         <v>23</v>
       </c>
       <c r="K23" s="24" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="L23" s="35" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="M23" s="24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N23" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="O23" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P23" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="Q23" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="R23" s="24"/>
       <c r="S23" s="34"/>
@@ -3745,17 +3866,17 @@
       <c r="U23" s="34"/>
       <c r="V23" s="34"/>
       <c r="W23" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="X23" s="34" t="s">
         <v>175</v>
-      </c>
-      <c r="X23" s="34" t="s">
-        <v>177</v>
       </c>
       <c r="Y23" s="34"/>
       <c r="Z23" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="AA23" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="AB23" s="7"/>
     </row>
@@ -3786,25 +3907,25 @@
         <v>23</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="L24" s="36" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="M24" s="24" t="s">
         <v>57</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="O24" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q24" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R24" s="24"/>
       <c r="S24" s="34"/>
@@ -3812,17 +3933,17 @@
       <c r="U24" s="34"/>
       <c r="V24" s="34"/>
       <c r="W24" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="X24" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Y24" s="34"/>
       <c r="Z24" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="AA24" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="AB24" s="7"/>
     </row>
@@ -3853,25 +3974,25 @@
         <v>23</v>
       </c>
       <c r="K25" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L25" s="37" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="M25" s="24" t="s">
         <v>57</v>
       </c>
       <c r="N25" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="O25" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P25" s="24" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="Q25" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="R25" s="24"/>
       <c r="S25" s="34"/>
@@ -3879,10 +4000,10 @@
       <c r="U25" s="34"/>
       <c r="V25" s="34"/>
       <c r="W25" s="34" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="X25" s="34" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="Y25" s="34"/>
       <c r="Z25" s="5"/>
@@ -3916,25 +4037,25 @@
         <v>23</v>
       </c>
       <c r="K26" s="24" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="L26" s="24" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="M26" s="24" t="s">
         <v>42</v>
       </c>
       <c r="N26" s="24" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="O26" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P26" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="Q26" s="24" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="R26" s="24"/>
       <c r="S26" s="34"/>
@@ -3942,14 +4063,14 @@
       <c r="U26" s="34"/>
       <c r="V26" s="34"/>
       <c r="W26" s="34" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="X26" s="34" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="Y26" s="34"/>
       <c r="Z26" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="AA26" s="5"/>
       <c r="AB26" s="7"/>
@@ -3976,16 +4097,16 @@
       <c r="L27" s="24"/>
       <c r="M27" s="24"/>
       <c r="N27" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="O27" s="24" t="s">
         <v>67</v>
       </c>
       <c r="P27" s="24" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="Q27" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="R27" s="24"/>
       <c r="S27" s="34"/>
@@ -3993,14 +4114,14 @@
       <c r="U27" s="34"/>
       <c r="V27" s="34"/>
       <c r="W27" s="34" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="X27" s="34" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="Y27" s="34"/>
       <c r="Z27" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="AA27" s="5"/>
       <c r="AB27" s="7"/>
@@ -4113,13 +4234,13 @@
     </row>
     <row r="30" spans="2:28" ht="180" x14ac:dyDescent="0.25">
       <c r="B30" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="C30" s="32" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="32" t="s">
         <v>194</v>
-      </c>
-      <c r="C30" s="32" t="s">
-        <v>195</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>196</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="32" t="s">
@@ -4141,16 +4262,16 @@
       <c r="L30" s="24"/>
       <c r="M30" s="24"/>
       <c r="N30" s="24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="O30" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P30" s="24" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="Q30" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="R30" s="24"/>
       <c r="S30" s="34"/>
@@ -4158,27 +4279,27 @@
       <c r="U30" s="34"/>
       <c r="V30" s="34"/>
       <c r="W30" s="34" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="X30" s="34" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="Y30" s="34"/>
       <c r="Z30" s="5"/>
       <c r="AA30" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="AB30" s="7"/>
     </row>
     <row r="31" spans="2:28" ht="180" x14ac:dyDescent="0.25">
       <c r="B31" s="32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C31" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D31" s="32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="32" t="s">
@@ -4200,16 +4321,16 @@
       <c r="L31" s="24"/>
       <c r="M31" s="24"/>
       <c r="N31" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="O31" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P31" s="24" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="Q31" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R31" s="24"/>
       <c r="S31" s="34"/>
@@ -4217,7 +4338,7 @@
       <c r="U31" s="34"/>
       <c r="V31" s="34"/>
       <c r="W31" s="34" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="X31" s="34"/>
       <c r="Y31" s="34"/>
@@ -4227,10 +4348,10 @@
     </row>
     <row r="32" spans="2:28" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="32" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C32" s="32" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D32" s="32"/>
       <c r="E32" s="32"/>
@@ -4249,16 +4370,16 @@
       <c r="L32" s="24"/>
       <c r="M32" s="24"/>
       <c r="N32" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="O32" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P32" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q32" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R32" s="24"/>
       <c r="S32" s="34"/>
@@ -4277,7 +4398,7 @@
         <v>17</v>
       </c>
       <c r="C33" s="32" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D33" s="32"/>
       <c r="E33" s="32"/>
@@ -4292,16 +4413,16 @@
       <c r="L33" s="24"/>
       <c r="M33" s="24"/>
       <c r="N33" s="24" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="O33" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P33" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="Q33" s="24" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="R33" s="24"/>
       <c r="S33" s="34"/>
@@ -4309,7 +4430,7 @@
       <c r="U33" s="34"/>
       <c r="V33" s="34"/>
       <c r="W33" s="34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="X33" s="34"/>
       <c r="Y33" s="34"/>
@@ -4322,10 +4443,10 @@
         <v>17</v>
       </c>
       <c r="C34" s="32" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D34" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E34" s="32"/>
       <c r="F34" s="32"/>
@@ -4341,16 +4462,16 @@
       <c r="L34" s="24"/>
       <c r="M34" s="24"/>
       <c r="N34" s="24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="O34" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P34" s="24" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="Q34" s="24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="R34" s="24"/>
       <c r="S34" s="34"/>
@@ -4358,27 +4479,27 @@
       <c r="U34" s="34"/>
       <c r="V34" s="34"/>
       <c r="W34" s="34" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="X34" s="34" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="Y34" s="34"/>
       <c r="Z34" s="5"/>
       <c r="AA34" s="5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="2:28" ht="225" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C35" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="D35" s="32" t="s">
         <v>223</v>
-      </c>
-      <c r="C35" s="32" t="s">
-        <v>224</v>
-      </c>
-      <c r="D35" s="32" t="s">
-        <v>225</v>
       </c>
       <c r="E35" s="32"/>
       <c r="F35" s="32" t="s">
@@ -4396,16 +4517,16 @@
       <c r="L35" s="24"/>
       <c r="M35" s="24"/>
       <c r="N35" s="24" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="O35" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P35" s="24" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="Q35" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="R35" s="24"/>
       <c r="S35" s="34"/>
@@ -4413,27 +4534,27 @@
       <c r="U35" s="34"/>
       <c r="V35" s="34"/>
       <c r="W35" s="34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="X35" s="34" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="Y35" s="34"/>
       <c r="Z35" s="5"/>
       <c r="AA35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="2:28" ht="285" x14ac:dyDescent="0.25">
       <c r="B36" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C36" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="D36" s="32" t="s">
         <v>223</v>
-      </c>
-      <c r="C36" s="32" t="s">
-        <v>232</v>
-      </c>
-      <c r="D36" s="32" t="s">
-        <v>225</v>
       </c>
       <c r="E36" s="32"/>
       <c r="F36" s="32" t="s">
@@ -4448,25 +4569,25 @@
         <v>13</v>
       </c>
       <c r="K36" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="L36" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="M36" s="24" t="s">
         <v>233</v>
       </c>
-      <c r="L36" s="24" t="s">
-        <v>234</v>
-      </c>
-      <c r="M36" s="24" t="s">
-        <v>235</v>
-      </c>
       <c r="N36" s="24" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="O36" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P36" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="Q36" s="24" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="R36" s="24"/>
       <c r="S36" s="34"/>
@@ -4474,13 +4595,13 @@
       <c r="U36" s="34"/>
       <c r="V36" s="34"/>
       <c r="W36" s="34" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="X36" s="34"/>
       <c r="Y36" s="34"/>
       <c r="Z36" s="5"/>
       <c r="AA36" s="5" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="AB36" s="7"/>
     </row>
@@ -4489,10 +4610,10 @@
         <v>17</v>
       </c>
       <c r="C37" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D37" s="32" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E37" s="32"/>
       <c r="F37" s="32" t="s">
@@ -4507,18 +4628,18 @@
         <v>13</v>
       </c>
       <c r="K37" s="24" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="L37" s="24"/>
       <c r="M37" s="24"/>
       <c r="N37" s="24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O37" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P37" s="24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="Q37" s="24"/>
       <c r="R37" s="24"/>
@@ -4527,7 +4648,7 @@
       <c r="U37" s="34"/>
       <c r="V37" s="34"/>
       <c r="W37" s="34" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="X37" s="34"/>
       <c r="Y37" s="34"/>
@@ -4540,10 +4661,10 @@
         <v>17</v>
       </c>
       <c r="C38" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D38" s="32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E38" s="32"/>
       <c r="F38" s="32" t="s">
@@ -4558,23 +4679,23 @@
         <v>13</v>
       </c>
       <c r="K38" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="L38" s="24" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="M38" s="24"/>
       <c r="N38" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O38" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P38" s="24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q38" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="R38" s="24"/>
       <c r="S38" s="34"/>
@@ -4593,10 +4714,10 @@
         <v>17</v>
       </c>
       <c r="C39" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D39" s="32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="32" t="s">
@@ -4611,23 +4732,23 @@
         <v>13</v>
       </c>
       <c r="K39" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="L39" s="24" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="M39" s="24"/>
       <c r="N39" s="24" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="O39" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P39" s="24" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="Q39" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="R39" s="24"/>
       <c r="S39" s="34"/>
@@ -4646,10 +4767,10 @@
         <v>17</v>
       </c>
       <c r="C40" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D40" s="32" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E40" s="32"/>
       <c r="F40" s="32" t="s">
@@ -4664,21 +4785,21 @@
         <v>13</v>
       </c>
       <c r="K40" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L40" s="24"/>
       <c r="M40" s="24"/>
       <c r="N40" s="24" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="O40" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P40" s="24" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="Q40" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="R40" s="24"/>
       <c r="S40" s="34"/>
@@ -4694,13 +4815,13 @@
     </row>
     <row r="41" spans="2:28" ht="135" x14ac:dyDescent="0.25">
       <c r="B41" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C41" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E41" s="32"/>
       <c r="F41" s="32" t="s">
@@ -4715,20 +4836,20 @@
         <v>13</v>
       </c>
       <c r="K41" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L41" s="24"/>
       <c r="M41" s="24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N41" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O41" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P41" s="24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Q41" s="24"/>
       <c r="R41" s="24"/>
@@ -4745,13 +4866,13 @@
     </row>
     <row r="42" spans="2:28" ht="105" x14ac:dyDescent="0.25">
       <c r="B42" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C42" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D42" s="32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E42" s="32"/>
       <c r="F42" s="32" t="s">
@@ -4766,20 +4887,20 @@
         <v>13</v>
       </c>
       <c r="K42" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L42" s="24"/>
       <c r="M42" s="24" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="N42" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O42" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P42" s="24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Q42" s="24"/>
       <c r="R42" s="24"/>
@@ -4796,13 +4917,13 @@
     </row>
     <row r="43" spans="2:28" ht="105" x14ac:dyDescent="0.25">
       <c r="B43" s="32" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C43" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D43" s="32" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="E43" s="32"/>
       <c r="F43" s="32" t="s">
@@ -4817,20 +4938,20 @@
         <v>13</v>
       </c>
       <c r="K43" s="24" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="L43" s="24"/>
       <c r="M43" s="24" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="N43" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="O43" s="24" t="s">
         <v>72</v>
       </c>
       <c r="P43" s="24" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="Q43" s="24"/>
       <c r="R43" s="24"/>
@@ -4872,20 +4993,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4862388-C0C2-40EF-9FDF-90ED8985F146}">
   <dimension ref="B2:X41"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" customWidth="1"/>
-    <col min="2" max="2" width="20.28515625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="9" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" style="9" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="9" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" style="9" customWidth="1"/>
     <col min="7" max="7" width="13.85546875" style="9" customWidth="1"/>
-    <col min="8" max="8" width="47.85546875" style="9" customWidth="1"/>
+    <col min="8" max="8" width="50.85546875" style="9" customWidth="1"/>
     <col min="9" max="9" width="11.140625" style="9" customWidth="1"/>
     <col min="10" max="11" width="13.140625" style="9" customWidth="1"/>
     <col min="12" max="12" width="8.140625" style="9" customWidth="1"/>
@@ -4902,18 +5024,18 @@
     <col min="23" max="24" width="9.140625" style="11"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:23" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>281</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>282</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>283</v>
-      </c>
-      <c r="J2" s="10" t="s">
-        <v>284</v>
       </c>
       <c r="K2" s="10"/>
       <c r="U2" s="10" t="s">
@@ -4922,86 +5044,106 @@
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="12" t="s">
+        <v>282</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>283</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>285</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="F3" s="12" t="s">
         <v>286</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>289</v>
       </c>
       <c r="G3" s="12" t="s">
         <v>8</v>
       </c>
       <c r="H3" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>289</v>
+      </c>
+      <c r="K3" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="L3" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="M3" s="15" t="s">
         <v>291</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="N3" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="K3" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="L3" s="14" t="s">
+      <c r="O3" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="M3" s="15" t="s">
+      <c r="P3" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="N3" s="15" t="s">
+      <c r="Q3" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="R3" s="18" t="s">
         <v>296</v>
       </c>
-      <c r="P3" s="16" t="s">
+      <c r="S3" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="Q3" s="17" t="s">
+      <c r="T3" s="20" t="s">
         <v>298</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="U3" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="V3" s="21" t="s">
         <v>300</v>
       </c>
-      <c r="T3" s="20" t="s">
-        <v>301</v>
-      </c>
-      <c r="U3" s="21" t="s">
-        <v>302</v>
-      </c>
-      <c r="V3" s="21" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+    </row>
+    <row r="4" spans="2:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
+      <c r="E4" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>310</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
+      <c r="K4" s="22" t="s">
+        <v>304</v>
+      </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
       <c r="O4" s="22"/>
-      <c r="P4" s="22"/>
-      <c r="Q4" s="22"/>
+      <c r="P4" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R4" s="22"/>
       <c r="S4" s="22"/>
       <c r="T4" s="23"/>
@@ -5010,22 +5152,42 @@
       <c r="W4" s="23"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
+      <c r="B5" s="22" t="s">
+        <v>309</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
+      <c r="E5" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
+      <c r="K5" s="22" t="s">
+        <v>304</v>
+      </c>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
       <c r="O5" s="22"/>
-      <c r="P5" s="22"/>
-      <c r="Q5" s="22"/>
+      <c r="P5" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R5" s="22"/>
       <c r="S5" s="22"/>
       <c r="T5" s="23"/>
@@ -5034,22 +5196,42 @@
       <c r="W5" s="23"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="22" t="s">
+        <v>313</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>314</v>
+      </c>
       <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
+      <c r="E6" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="K6" s="22" t="s">
+        <v>304</v>
+      </c>
       <c r="L6" s="22"/>
       <c r="M6" s="22"/>
       <c r="N6" s="22"/>
       <c r="O6" s="22"/>
-      <c r="P6" s="22"/>
-      <c r="Q6" s="22"/>
+      <c r="P6" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R6" s="22"/>
       <c r="S6" s="22"/>
       <c r="T6" s="23"/>
@@ -5058,22 +5240,42 @@
       <c r="W6" s="23"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
+      <c r="B7" s="22" t="s">
+        <v>315</v>
+      </c>
+      <c r="C7" s="22" t="s">
+        <v>316</v>
+      </c>
       <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
-      <c r="I7" s="22"/>
+      <c r="E7" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>311</v>
+      </c>
+      <c r="I7" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J7" s="22"/>
-      <c r="K7" s="22"/>
+      <c r="K7" s="22" t="s">
+        <v>304</v>
+      </c>
       <c r="L7" s="22"/>
       <c r="M7" s="22"/>
       <c r="N7" s="22"/>
       <c r="O7" s="22"/>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
+      <c r="P7" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R7" s="22"/>
       <c r="S7" s="22"/>
       <c r="T7" s="23"/>
@@ -5081,23 +5283,43 @@
       <c r="V7" s="23"/>
       <c r="W7" s="23"/>
     </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
+    <row r="8" spans="2:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="B8" s="22" t="s">
+        <v>318</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>319</v>
+      </c>
       <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
+      <c r="E8" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="I8" s="22" t="s">
+        <v>321</v>
+      </c>
       <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
+      <c r="K8" s="22" t="s">
+        <v>304</v>
+      </c>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
       <c r="N8" s="22"/>
       <c r="O8" s="22"/>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
+      <c r="P8" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
       <c r="T8" s="23"/>
@@ -5105,23 +5327,45 @@
       <c r="V8" s="23"/>
       <c r="W8" s="23"/>
     </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
+    <row r="9" spans="2:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="B9" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>319</v>
+      </c>
       <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
+      <c r="E9" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="I9" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J9" s="22"/>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
+      <c r="K9" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>20</v>
+      </c>
       <c r="M9" s="22"/>
       <c r="N9" s="22"/>
       <c r="O9" s="22"/>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
+      <c r="P9" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R9" s="22"/>
       <c r="S9" s="22"/>
       <c r="T9" s="23"/>
@@ -5129,23 +5373,43 @@
       <c r="V9" s="23"/>
       <c r="W9" s="23"/>
     </row>
-    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
+    <row r="10" spans="2:23" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
+      <c r="E10" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="I10" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
+      <c r="K10" s="22" t="s">
+        <v>328</v>
+      </c>
       <c r="L10" s="22"/>
       <c r="M10" s="22"/>
       <c r="N10" s="22"/>
       <c r="O10" s="22"/>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
+      <c r="P10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R10" s="22"/>
       <c r="S10" s="22"/>
       <c r="T10" s="23"/>
@@ -5153,23 +5417,43 @@
       <c r="V10" s="23"/>
       <c r="W10" s="23"/>
     </row>
-    <row r="11" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
+    <row r="11" spans="2:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="B11" s="22" t="s">
+        <v>330</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>86</v>
+      </c>
       <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="22"/>
+      <c r="E11" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="I11" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J11" s="22"/>
-      <c r="K11" s="22"/>
+      <c r="K11" s="22" t="s">
+        <v>328</v>
+      </c>
       <c r="L11" s="22"/>
       <c r="M11" s="22"/>
       <c r="N11" s="22"/>
       <c r="O11" s="22"/>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
+      <c r="P11" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R11" s="22"/>
       <c r="S11" s="22"/>
       <c r="T11" s="23"/>
@@ -5177,23 +5461,43 @@
       <c r="V11" s="23"/>
       <c r="W11" s="23"/>
     </row>
-    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+    <row r="12" spans="2:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>314</v>
+      </c>
       <c r="D12" s="22"/>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
+      <c r="E12" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="I12" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
+      <c r="K12" s="22" t="s">
+        <v>328</v>
+      </c>
       <c r="L12" s="22"/>
       <c r="M12" s="22"/>
       <c r="N12" s="22"/>
       <c r="O12" s="22"/>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
+      <c r="P12" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q12" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R12" s="22"/>
       <c r="S12" s="22"/>
       <c r="T12" s="23"/>
@@ -5201,23 +5505,43 @@
       <c r="V12" s="23"/>
       <c r="W12" s="23"/>
     </row>
-    <row r="13" spans="2:23" x14ac:dyDescent="0.25">
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
+    <row r="13" spans="2:23" ht="60" x14ac:dyDescent="0.25">
+      <c r="B13" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>316</v>
+      </c>
       <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
+      <c r="E13" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>334</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>312</v>
+      </c>
       <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
+      <c r="K13" s="22" t="s">
+        <v>328</v>
+      </c>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
       <c r="N13" s="22"/>
       <c r="O13" s="22"/>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
+      <c r="P13" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>317</v>
+      </c>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
       <c r="T13" s="23"/>

</xml_diff>